<commit_message>
Add different levels of users
</commit_message>
<xml_diff>
--- a/bin/files/users.xlsx
+++ b/bin/files/users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/treycarey/Documents/GitHub/Lower Thirds SDV/resources/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F1396C0-3633-8A4A-A023-DD9EC6982E52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC0DFEE2-35D1-D140-901B-8CD8DF5C2A5F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14180" xr2:uid="{587F98F7-21DC-4C4A-B441-EFBDC8FE4D6A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>NAME</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>Samuel Lopez</t>
+  </si>
+  <si>
+    <t>password123</t>
   </si>
 </sst>
 </file>
@@ -420,13 +423,13 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="12.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="13" style="1" customWidth="1"/>
     <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
@@ -457,6 +460,9 @@
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="C3" s="1">
         <v>3</v>
       </c>
@@ -465,6 +471,9 @@
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="C4" s="1">
         <v>3</v>
       </c>
@@ -473,13 +482,19 @@
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="C5" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="C6" s="1">
         <v>3</v>

</xml_diff>

<commit_message>
Bugfix and small refactoring
</commit_message>
<xml_diff>
--- a/bin/files/users.xlsx
+++ b/bin/files/users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/treycarey/Documents/GitHub/Lower Thirds SDV/resources/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC0DFEE2-35D1-D140-901B-8CD8DF5C2A5F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1387DEC-CBD9-7B47-B35A-F97031882D98}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14180" xr2:uid="{587F98F7-21DC-4C4A-B441-EFBDC8FE4D6A}"/>
   </bookViews>
@@ -423,7 +423,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -458,7 +458,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
@@ -469,35 +469,35 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Basic Dashboard Background Added, Minor Refactoring
Cleaned up some if statements and made some code optimizations
</commit_message>
<xml_diff>
--- a/bin/files/users.xlsx
+++ b/bin/files/users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/treycarey/Documents/GitHub/Lower Thirds SDV/resources/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1387DEC-CBD9-7B47-B35A-F97031882D98}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B4A326-974B-7F4E-BC5C-B4BF09BEAB2E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14180" xr2:uid="{587F98F7-21DC-4C4A-B441-EFBDC8FE4D6A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>NAME</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>password123</t>
+  </si>
+  <si>
+    <t>USERNAME</t>
   </si>
 </sst>
 </file>
@@ -420,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1639D595-554F-BA4A-B9B2-83799418169C}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -500,6 +503,17 @@
         <v>2</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed SD not changing screens
Bugs only seem to occur when no second display is plugged in, weird.
</commit_message>
<xml_diff>
--- a/bin/files/users.xlsx
+++ b/bin/files/users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/treycarey/Documents/GitHub/Lower Thirds SDV/resources/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E85407B5-55BE-9E43-A2E1-A15370FFCDE1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF0C04D-5BCC-8640-A9A2-2D0EA43F49E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14180" xr2:uid="{587F98F7-21DC-4C4A-B441-EFBDC8FE4D6A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
   <si>
     <t>NAME</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Kevin Blenman</t>
+  </si>
+  <si>
+    <t>USERNAME</t>
   </si>
 </sst>
 </file>
@@ -423,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1639D595-554F-BA4A-B9B2-83799418169C}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -514,6 +517,17 @@
         <v>1</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Options in Admin Settings
</commit_message>
<xml_diff>
--- a/bin/files/users.xlsx
+++ b/bin/files/users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/treycarey/Documents/GitHub/Lower Thirds SDV/resources/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415240A8-7D61-8347-86E3-5F401C3220F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE065E52-1FD3-054A-8DC3-98EEBAEAD5A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14180" xr2:uid="{587F98F7-21DC-4C4A-B441-EFBDC8FE4D6A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>NAME</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>T2002Carey</t>
+  </si>
+  <si>
+    <t>tigers</t>
   </si>
 </sst>
 </file>
@@ -442,7 +445,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -524,7 +527,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>

</xml_diff>